<commit_message>
10042025 sampling data entered
</commit_message>
<xml_diff>
--- a/F25_Sampling.xlsx
+++ b/F25_Sampling.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trini/Documents/Shedd/Cruise_Sep_2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trini/Documents/Shedd/biota_project_genomicshifts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE830FB-4C92-134C-A06D-494842F91C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47085EA2-3DCE-5742-B98E-19B6D086D68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5320" yWindow="1880" windowWidth="24040" windowHeight="12440" activeTab="1" xr2:uid="{07AAFEEF-A83C-484C-8992-E89847C75F27}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="template" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1557,31 +1557,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -1925,7 +1920,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -2379,503 +2374,53 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-    </row>
-    <row r="41" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-    </row>
-    <row r="55" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-    </row>
-    <row r="59" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-    </row>
-    <row r="61" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-    </row>
-    <row r="62" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-    </row>
-    <row r="63" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-    </row>
-    <row r="64" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-    </row>
-    <row r="65" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-    </row>
-    <row r="66" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-    </row>
-    <row r="67" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-    </row>
-    <row r="68" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-    </row>
-    <row r="70" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-    </row>
-    <row r="71" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-    </row>
-    <row r="74" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-    </row>
-    <row r="75" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-    </row>
-    <row r="77" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-    </row>
-    <row r="78" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-    </row>
-    <row r="79" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-    </row>
-    <row r="80" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-    </row>
-    <row r="81" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-    </row>
+    <row r="35" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -2886,8 +2431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859618DA-7D2E-F14A-9531-A0F7323C3157}">
   <dimension ref="A1:P257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J105" sqref="J105"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J114" sqref="J114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2896,42 +2441,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -2940,10 +2485,10 @@
       <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2">
         <v>1564</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" t="s">
         <v>24</v>
       </c>
       <c r="F2" t="s">
@@ -2960,7 +2505,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>60</v>
       </c>
       <c r="B3" t="s">
@@ -2969,13 +2514,13 @@
       <c r="C3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3">
         <v>1566</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" t="s">
         <v>67</v>
       </c>
       <c r="G3">
@@ -2990,19 +2535,19 @@
       <c r="J3">
         <v>50</v>
       </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="15" t="s">
+      <c r="M3" s="8"/>
+      <c r="N3" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="16" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>62</v>
       </c>
       <c r="B4" t="s">
@@ -3011,13 +2556,13 @@
       <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4">
         <v>1566</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" t="s">
         <v>67</v>
       </c>
       <c r="G4">
@@ -3035,24 +2580,24 @@
       <c r="K4" t="s">
         <v>74</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="20">
         <f>COUNTIFS(C:C, "Cnat")</f>
         <v>37</v>
       </c>
-      <c r="O4" s="17">
+      <c r="O4" s="12">
         <f>COUNTIFS(C:C,"Cnat", F:F, "Y" )</f>
         <v>8</v>
       </c>
-      <c r="P4" s="22">
+      <c r="P4" s="17">
         <f>COUNTIFS(C:C,"Cnat", F:F, "N" )</f>
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>66</v>
       </c>
       <c r="B5" t="s">
@@ -3082,24 +2627,24 @@
       <c r="K5" t="s">
         <v>77</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="M5" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="N5" s="26">
+      <c r="N5" s="21">
         <f>COUNTIFS(C:C, "Dlab")</f>
         <v>26</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="13">
         <f>COUNTIFS(C:C,"Dlab", F:F, "Y" )</f>
         <v>3</v>
       </c>
-      <c r="P5" s="23">
+      <c r="P5" s="18">
         <f>COUNTIFS(C:C,"Dlab", F:F, "N" )</f>
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>105</v>
       </c>
       <c r="B6" t="s">
@@ -3126,24 +2671,24 @@
       <c r="J6">
         <v>51</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="21">
         <f>COUNTIFS(C:C,"Mcav")</f>
         <v>51</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="13">
         <f>COUNTIFS(C:C,"Mcav", F:F, "Y" )</f>
         <v>20</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="18">
         <f>COUNTIFS(C:C,"Mcav", F:F, "N" )</f>
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>77</v>
       </c>
       <c r="B7" t="s">
@@ -3170,24 +2715,24 @@
       <c r="J7">
         <v>56</v>
       </c>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N7" s="26">
+      <c r="N7" s="21">
         <f>COUNTIFS(C:C, "Sint")</f>
         <v>38</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="14">
         <f>COUNTIFS(C:C,"Sint", F:F, "Y" )</f>
         <v>13</v>
       </c>
-      <c r="P7" s="23">
+      <c r="P7" s="18">
         <f>COUNTIFS(C:C,"Sint", F:F, "N" )</f>
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -3196,13 +2741,13 @@
       <c r="C8" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8">
         <v>1564</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" t="s">
         <v>66</v>
       </c>
       <c r="G8">
@@ -3217,24 +2762,24 @@
       <c r="K8" t="s">
         <v>68</v>
       </c>
-      <c r="M8" s="27" t="s">
+      <c r="M8" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="N8" s="26">
+      <c r="N8" s="21">
         <f>COUNTIFS(C:C, "Past")</f>
         <v>32</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="13">
         <f>COUNTIFS(C:C,"Past", F:F, "Y" )</f>
         <v>14</v>
       </c>
-      <c r="P8" s="23">
+      <c r="P8" s="18">
         <f>COUNTIFS(C:C,"Past", F:F, "N" )</f>
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>54</v>
       </c>
       <c r="B9" t="s">
@@ -3243,13 +2788,13 @@
       <c r="C9" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9">
         <v>1566</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" t="s">
         <v>66</v>
       </c>
       <c r="G9">
@@ -3264,24 +2809,24 @@
       <c r="J9">
         <v>51</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="N9" s="26">
+      <c r="N9" s="21">
         <f>COUNTIFS(C:C, "Pstr")</f>
         <v>30</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="13">
         <f>COUNTIFS(C:C,"Pstr", F:F, "Y" )</f>
         <v>9</v>
       </c>
-      <c r="P9" s="23">
+      <c r="P9" s="18">
         <f>COUNTIFS(C:C,"Pstr", F:F, "N" )</f>
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>115</v>
       </c>
       <c r="B10" t="s">
@@ -3308,24 +2853,24 @@
       <c r="J10">
         <v>54</v>
       </c>
-      <c r="M10" s="27" t="s">
+      <c r="M10" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="N10" s="26">
+      <c r="N10" s="21">
         <f>COUNTIFS(C:C, "Ssid")</f>
         <v>38</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="13">
         <f>COUNTIFS(C:C,"Ssid", F:F, "Y" )</f>
         <v>12</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="18">
         <f>COUNTIFS(C:C,"Ssid", F:F, "N" )</f>
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>76</v>
       </c>
       <c r="B11" t="s">
@@ -3352,16 +2897,16 @@
       <c r="J11">
         <v>56</v>
       </c>
-      <c r="M11" s="14"/>
-      <c r="N11" s="11">
+      <c r="M11" s="9"/>
+      <c r="N11" s="6">
         <f>SUM(N4:N10)</f>
         <v>252</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="24"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="19"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>78</v>
       </c>
       <c r="B12" t="s">
@@ -3390,7 +2935,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>79</v>
       </c>
       <c r="B13" t="s">
@@ -3419,7 +2964,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>35</v>
       </c>
       <c r="B14" t="s">
@@ -3445,7 +2990,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" t="s">
@@ -3454,10 +2999,10 @@
       <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15">
         <v>1564</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" t="s">
         <v>24</v>
       </c>
       <c r="F15" t="s">
@@ -3474,7 +3019,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>5</v>
       </c>
       <c r="B16" t="s">
@@ -3483,10 +3028,10 @@
       <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16">
         <v>1564</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" t="s">
         <v>24</v>
       </c>
       <c r="F16" t="s">
@@ -3503,7 +3048,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17">
         <v>9</v>
       </c>
       <c r="B17" t="s">
@@ -3512,10 +3057,10 @@
       <c r="C17" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17">
         <v>1564</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" t="s">
         <v>24</v>
       </c>
       <c r="F17" t="s">
@@ -3532,7 +3077,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18">
         <v>53</v>
       </c>
       <c r="B18" t="s">
@@ -3541,13 +3086,13 @@
       <c r="C18" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18">
         <v>1566</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" t="s">
         <v>67</v>
       </c>
       <c r="G18">
@@ -3564,7 +3109,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19">
         <v>57</v>
       </c>
       <c r="B19" t="s">
@@ -3573,13 +3118,13 @@
       <c r="C19" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19">
         <v>1566</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" t="s">
         <v>67</v>
       </c>
       <c r="G19">
@@ -3596,7 +3141,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20">
         <v>63</v>
       </c>
       <c r="B20" t="s">
@@ -3605,13 +3150,13 @@
       <c r="C20" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>1566</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" t="s">
         <v>66</v>
       </c>
       <c r="G20">
@@ -3628,7 +3173,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="A21">
         <v>102</v>
       </c>
       <c r="B21" t="s">
@@ -3660,7 +3205,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22">
         <v>67</v>
       </c>
       <c r="B22" t="s">
@@ -3692,7 +3237,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23">
         <v>104</v>
       </c>
       <c r="B23" t="s">
@@ -3724,7 +3269,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24">
         <v>119</v>
       </c>
       <c r="B24" t="s">
@@ -3753,7 +3298,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25">
         <v>145</v>
       </c>
       <c r="B25" t="s">
@@ -3782,7 +3327,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26">
         <v>71</v>
       </c>
       <c r="B26" t="s">
@@ -3811,7 +3356,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+      <c r="A27">
         <v>75</v>
       </c>
       <c r="B27" t="s">
@@ -3840,7 +3385,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28">
         <v>149</v>
       </c>
       <c r="B28" t="s">
@@ -3869,7 +3414,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+      <c r="A29">
         <v>153</v>
       </c>
       <c r="B29" t="s">
@@ -3898,7 +3443,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+      <c r="A30">
         <v>156</v>
       </c>
       <c r="B30" t="s">
@@ -3927,7 +3472,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+      <c r="A31">
         <v>157</v>
       </c>
       <c r="B31" t="s">
@@ -3956,7 +3501,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
+      <c r="A32">
         <v>37</v>
       </c>
       <c r="B32" t="s">
@@ -3982,7 +3527,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
+      <c r="A33">
         <v>47</v>
       </c>
       <c r="B33" t="s">
@@ -4008,7 +3553,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
+      <c r="A34">
         <v>21</v>
       </c>
       <c r="B34" t="s">
@@ -4037,7 +3582,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+      <c r="A35">
         <v>26</v>
       </c>
       <c r="B35" t="s">
@@ -4063,7 +3608,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
+      <c r="A36">
         <v>31</v>
       </c>
       <c r="B36" t="s">
@@ -4089,38 +3634,38 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
+      <c r="A37" s="3">
         <v>1</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="3">
         <v>1564</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" s="6">
-        <v>20251002</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6">
+      <c r="F37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="3">
+        <v>20251002</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3">
         <v>54</v>
       </c>
-      <c r="K37" s="6"/>
+      <c r="K37" s="3"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
+      <c r="A38">
         <v>20</v>
       </c>
       <c r="B38" t="s">
@@ -4146,7 +3691,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+      <c r="A39">
         <v>2</v>
       </c>
       <c r="B39" t="s">
@@ -4155,10 +3700,10 @@
       <c r="C39" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39">
         <v>1564</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" t="s">
         <v>24</v>
       </c>
       <c r="F39" t="s">
@@ -4175,7 +3720,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
+      <c r="A40">
         <v>8</v>
       </c>
       <c r="B40" t="s">
@@ -4184,10 +3729,10 @@
       <c r="C40" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40">
         <v>1564</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" t="s">
         <v>24</v>
       </c>
       <c r="F40" t="s">
@@ -4204,7 +3749,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
+      <c r="A41">
         <v>55</v>
       </c>
       <c r="B41" t="s">
@@ -4213,13 +3758,13 @@
       <c r="C41" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41">
         <v>1566</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" t="s">
         <v>82</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" t="s">
         <v>67</v>
       </c>
       <c r="G41">
@@ -4236,7 +3781,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
+      <c r="A42">
         <v>69</v>
       </c>
       <c r="B42" t="s">
@@ -4268,7 +3813,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
+      <c r="A43">
         <v>70</v>
       </c>
       <c r="B43" t="s">
@@ -4297,7 +3842,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
+      <c r="A44">
         <v>90</v>
       </c>
       <c r="B44" t="s">
@@ -4329,7 +3874,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
+      <c r="A45">
         <v>36</v>
       </c>
       <c r="B45" t="s">
@@ -4355,7 +3900,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
+      <c r="A46">
         <v>42</v>
       </c>
       <c r="B46" t="s">
@@ -4381,7 +3926,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
+      <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
@@ -4407,7 +3952,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
+      <c r="A48">
         <v>19</v>
       </c>
       <c r="B48" t="s">
@@ -4433,7 +3978,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+      <c r="A49">
         <v>25</v>
       </c>
       <c r="B49" t="s">
@@ -4459,7 +4004,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
+      <c r="A50">
         <v>27</v>
       </c>
       <c r="B50" t="s">
@@ -4488,7 +4033,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+      <c r="A51">
         <v>30</v>
       </c>
       <c r="B51" t="s">
@@ -4514,7 +4059,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+      <c r="A52">
         <v>13</v>
       </c>
       <c r="B52" t="s">
@@ -4523,10 +4068,10 @@
       <c r="C52" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52">
         <v>1564</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E52" t="s">
         <v>24</v>
       </c>
       <c r="F52" t="s">
@@ -4546,7 +4091,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+      <c r="A53">
         <v>15</v>
       </c>
       <c r="B53" t="s">
@@ -4555,10 +4100,10 @@
       <c r="C53" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53">
         <v>1564</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" t="s">
         <v>24</v>
       </c>
       <c r="F53" t="s">
@@ -4575,7 +4120,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
+      <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
@@ -4584,13 +4129,13 @@
       <c r="C54" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54">
         <v>1566</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="E54" t="s">
         <v>79</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F54" t="s">
         <v>66</v>
       </c>
       <c r="G54">
@@ -4610,7 +4155,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="7">
+      <c r="A55" s="4">
         <v>61</v>
       </c>
       <c r="B55" t="s">
@@ -4619,13 +4164,13 @@
       <c r="C55" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55">
         <v>1566</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" t="s">
         <v>86</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="F55" t="s">
         <v>66</v>
       </c>
       <c r="G55">
@@ -4642,7 +4187,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
+      <c r="A56">
         <v>68</v>
       </c>
       <c r="B56" t="s">
@@ -4671,7 +4216,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
+      <c r="A57">
         <v>72</v>
       </c>
       <c r="B57" t="s">
@@ -4700,7 +4245,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
+      <c r="A58">
         <v>92</v>
       </c>
       <c r="B58" t="s">
@@ -4729,7 +4274,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="4">
+      <c r="A59">
         <v>143</v>
       </c>
       <c r="B59" t="s">
@@ -4758,7 +4303,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="4">
+      <c r="A60">
         <v>109</v>
       </c>
       <c r="B60" t="s">
@@ -4790,7 +4335,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" s="4">
+      <c r="A61">
         <v>151</v>
       </c>
       <c r="B61" t="s">
@@ -4819,7 +4364,7 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" s="4">
+      <c r="A62">
         <v>152</v>
       </c>
       <c r="B62" t="s">
@@ -4848,7 +4393,7 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="4">
+      <c r="A63">
         <v>155</v>
       </c>
       <c r="B63" t="s">
@@ -4877,7 +4422,7 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="4">
+      <c r="A64">
         <v>34</v>
       </c>
       <c r="B64" t="s">
@@ -4903,7 +4448,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" s="4">
+      <c r="A65">
         <v>40</v>
       </c>
       <c r="B65" t="s">
@@ -4929,7 +4474,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" s="4">
+      <c r="A66">
         <v>38</v>
       </c>
       <c r="B66" t="s">
@@ -4955,7 +4500,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="4">
+      <c r="A67">
         <v>49</v>
       </c>
       <c r="B67" t="s">
@@ -4981,7 +4526,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
+      <c r="A68">
         <v>22</v>
       </c>
       <c r="B68" t="s">
@@ -5007,7 +4552,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="4">
+      <c r="A69">
         <v>24</v>
       </c>
       <c r="B69" t="s">
@@ -5033,7 +4578,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="4">
+      <c r="A70">
         <v>41</v>
       </c>
       <c r="B70" t="s">
@@ -5059,7 +4604,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="4">
+      <c r="A71">
         <v>7</v>
       </c>
       <c r="B71" t="s">
@@ -5068,10 +4613,10 @@
       <c r="C71" t="s">
         <v>62</v>
       </c>
-      <c r="D71" s="9">
+      <c r="D71">
         <v>1564</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="E71" t="s">
         <v>24</v>
       </c>
       <c r="F71" t="s">
@@ -5088,7 +4633,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="4">
+      <c r="A72">
         <v>12</v>
       </c>
       <c r="B72" t="s">
@@ -5097,10 +4642,10 @@
       <c r="C72" t="s">
         <v>62</v>
       </c>
-      <c r="D72" s="9">
+      <c r="D72">
         <v>1564</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="E72" t="s">
         <v>24</v>
       </c>
       <c r="F72" t="s">
@@ -5117,40 +4662,40 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="5">
+      <c r="A73" s="3">
         <v>16</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73" s="3">
         <v>1564</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="E73" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F73" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G73" s="6">
-        <v>20251002</v>
-      </c>
-      <c r="H73" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I73" s="6"/>
-      <c r="J73" s="6">
+      <c r="F73" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G73" s="3">
+        <v>20251002</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3">
         <v>54</v>
       </c>
-      <c r="K73" s="6" t="s">
+      <c r="K73" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="4">
+      <c r="A74">
         <v>56</v>
       </c>
       <c r="B74" t="s">
@@ -5159,13 +4704,13 @@
       <c r="C74" t="s">
         <v>62</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74">
         <v>1566</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E74" t="s">
         <v>83</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="F74" t="s">
         <v>66</v>
       </c>
       <c r="G74">
@@ -5182,7 +4727,7 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="4">
+      <c r="A75">
         <v>59</v>
       </c>
       <c r="B75" t="s">
@@ -5191,13 +4736,13 @@
       <c r="C75" t="s">
         <v>62</v>
       </c>
-      <c r="D75" s="9">
+      <c r="D75">
         <v>1566</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E75" t="s">
         <v>85</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F75" t="s">
         <v>66</v>
       </c>
       <c r="G75">
@@ -5214,7 +4759,7 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="4">
+      <c r="A76">
         <v>65</v>
       </c>
       <c r="B76" t="s">
@@ -5243,7 +4788,7 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" s="4">
+      <c r="A77">
         <v>120</v>
       </c>
       <c r="B77" t="s">
@@ -5272,7 +4817,7 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="4">
+      <c r="A78">
         <v>74</v>
       </c>
       <c r="B78" t="s">
@@ -5301,7 +4846,7 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="4">
+      <c r="A79">
         <v>150</v>
       </c>
       <c r="B79" t="s">
@@ -5330,7 +4875,7 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="4">
+      <c r="A80">
         <v>126</v>
       </c>
       <c r="B80" t="s">
@@ -5359,7 +4904,7 @@
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" s="4">
+      <c r="A81">
         <v>33</v>
       </c>
       <c r="B81" t="s">
@@ -5385,7 +4930,7 @@
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="4">
+      <c r="A82">
         <v>39</v>
       </c>
       <c r="B82" t="s">
@@ -5411,7 +4956,7 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="4">
+      <c r="A83">
         <v>45</v>
       </c>
       <c r="B83" t="s">
@@ -5437,7 +4982,7 @@
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" s="4">
+      <c r="A84">
         <v>48</v>
       </c>
       <c r="B84" t="s">
@@ -5463,7 +5008,7 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" s="4">
+      <c r="A85">
         <v>28</v>
       </c>
       <c r="B85" t="s">
@@ -5492,7 +5037,7 @@
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A86" s="4">
+      <c r="A86">
         <v>52</v>
       </c>
       <c r="B86" t="s">
@@ -5518,7 +5063,7 @@
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A87" s="4">
+      <c r="A87">
         <v>130</v>
       </c>
       <c r="B87" t="s">
@@ -5550,7 +5095,7 @@
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" s="4">
+      <c r="A88">
         <v>4</v>
       </c>
       <c r="B88" t="s">
@@ -5559,10 +5104,10 @@
       <c r="C88" t="s">
         <v>61</v>
       </c>
-      <c r="D88" s="9">
+      <c r="D88">
         <v>1564</v>
       </c>
-      <c r="E88" s="9" t="s">
+      <c r="E88" t="s">
         <v>24</v>
       </c>
       <c r="F88" t="s">
@@ -5579,7 +5124,7 @@
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" s="4">
+      <c r="A89">
         <v>6</v>
       </c>
       <c r="B89" t="s">
@@ -5588,10 +5133,10 @@
       <c r="C89" t="s">
         <v>61</v>
       </c>
-      <c r="D89" s="9">
+      <c r="D89">
         <v>1564</v>
       </c>
-      <c r="E89" s="9" t="s">
+      <c r="E89" t="s">
         <v>24</v>
       </c>
       <c r="F89" t="s">
@@ -5608,7 +5153,7 @@
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90" s="4">
+      <c r="A90">
         <v>10</v>
       </c>
       <c r="B90" t="s">
@@ -5617,10 +5162,10 @@
       <c r="C90" t="s">
         <v>61</v>
       </c>
-      <c r="D90" s="9">
+      <c r="D90">
         <v>1564</v>
       </c>
-      <c r="E90" s="9" t="s">
+      <c r="E90" t="s">
         <v>24</v>
       </c>
       <c r="F90" t="s">
@@ -5637,7 +5182,7 @@
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A91" s="4">
+      <c r="A91">
         <v>11</v>
       </c>
       <c r="B91" t="s">
@@ -5646,10 +5191,10 @@
       <c r="C91" t="s">
         <v>61</v>
       </c>
-      <c r="D91" s="9">
+      <c r="D91">
         <v>1564</v>
       </c>
-      <c r="E91" s="9" t="s">
+      <c r="E91" t="s">
         <v>24</v>
       </c>
       <c r="F91" t="s">
@@ -5666,7 +5211,7 @@
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" s="4">
+      <c r="A92">
         <v>51</v>
       </c>
       <c r="B92" t="s">
@@ -5675,13 +5220,13 @@
       <c r="C92" t="s">
         <v>61</v>
       </c>
-      <c r="D92" s="9">
+      <c r="D92">
         <v>1566</v>
       </c>
-      <c r="E92" s="9" t="s">
+      <c r="E92" t="s">
         <v>78</v>
       </c>
-      <c r="F92" s="9" t="s">
+      <c r="F92" t="s">
         <v>66</v>
       </c>
       <c r="G92">
@@ -5698,7 +5243,7 @@
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" s="4">
+      <c r="A93">
         <v>58</v>
       </c>
       <c r="B93" t="s">
@@ -5707,13 +5252,13 @@
       <c r="C93" t="s">
         <v>61</v>
       </c>
-      <c r="D93" s="9">
+      <c r="D93">
         <v>1566</v>
       </c>
-      <c r="E93" s="9" t="s">
+      <c r="E93" t="s">
         <v>80</v>
       </c>
-      <c r="F93" s="9" t="s">
+      <c r="F93" t="s">
         <v>67</v>
       </c>
       <c r="G93">
@@ -5730,7 +5275,7 @@
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="4">
+      <c r="A94">
         <v>101</v>
       </c>
       <c r="B94" t="s">
@@ -5762,7 +5307,7 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="4">
+      <c r="A95">
         <v>64</v>
       </c>
       <c r="B95" t="s">
@@ -5794,7 +5339,7 @@
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" s="4">
+      <c r="A96">
         <v>106</v>
       </c>
       <c r="B96" t="s">
@@ -5823,7 +5368,7 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A97" s="4">
+      <c r="A97">
         <v>73</v>
       </c>
       <c r="B97" t="s">
@@ -5852,7 +5397,7 @@
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="4">
+      <c r="A98">
         <v>91</v>
       </c>
       <c r="B98" t="s">
@@ -5881,7 +5426,7 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A99" s="4">
+      <c r="A99">
         <v>154</v>
       </c>
       <c r="B99" t="s">
@@ -5910,7 +5455,7 @@
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A100" s="4">
+      <c r="A100">
         <v>43</v>
       </c>
       <c r="B100" t="s">
@@ -5936,7 +5481,7 @@
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A101" s="4">
+      <c r="A101">
         <v>44</v>
       </c>
       <c r="B101" t="s">
@@ -5962,7 +5507,7 @@
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A102" s="4">
+      <c r="A102">
         <v>18</v>
       </c>
       <c r="B102" t="s">
@@ -5988,7 +5533,7 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A103" s="4">
+      <c r="A103">
         <v>23</v>
       </c>
       <c r="B103" t="s">
@@ -6014,7 +5559,7 @@
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A104" s="4">
+      <c r="A104">
         <v>29</v>
       </c>
       <c r="B104" t="s">
@@ -6043,7 +5588,7 @@
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A105" s="4">
+      <c r="A105">
         <v>201</v>
       </c>
       <c r="B105" t="s">
@@ -6067,9 +5612,12 @@
       <c r="H105" t="s">
         <v>188</v>
       </c>
+      <c r="J105">
+        <v>20</v>
+      </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A106" s="4">
+      <c r="A106">
         <v>202</v>
       </c>
       <c r="B106" t="s">
@@ -6093,9 +5641,12 @@
       <c r="H106" t="s">
         <v>188</v>
       </c>
+      <c r="J106">
+        <v>25</v>
+      </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A107" s="4">
+      <c r="A107">
         <v>203</v>
       </c>
       <c r="B107" t="s">
@@ -6119,9 +5670,12 @@
       <c r="H107" t="s">
         <v>188</v>
       </c>
+      <c r="J107">
+        <v>26</v>
+      </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A108" s="4">
+      <c r="A108">
         <v>204</v>
       </c>
       <c r="B108" t="s">
@@ -6145,9 +5699,12 @@
       <c r="H108" t="s">
         <v>188</v>
       </c>
+      <c r="J108">
+        <v>24</v>
+      </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A109" s="4">
+      <c r="A109">
         <v>205</v>
       </c>
       <c r="B109" t="s">
@@ -6171,9 +5728,12 @@
       <c r="H109" t="s">
         <v>188</v>
       </c>
+      <c r="J109">
+        <v>25</v>
+      </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A110" s="4">
+      <c r="A110">
         <v>206</v>
       </c>
       <c r="B110" t="s">
@@ -6197,9 +5757,12 @@
       <c r="H110" t="s">
         <v>188</v>
       </c>
+      <c r="J110">
+        <v>25</v>
+      </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A111" s="4">
+      <c r="A111">
         <v>207</v>
       </c>
       <c r="B111" t="s">
@@ -6223,9 +5786,12 @@
       <c r="H111" t="s">
         <v>188</v>
       </c>
+      <c r="J111">
+        <v>26</v>
+      </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A112" s="4">
+      <c r="A112">
         <v>208</v>
       </c>
       <c r="B112" t="s">
@@ -6249,9 +5815,12 @@
       <c r="H112" t="s">
         <v>188</v>
       </c>
+      <c r="J112">
+        <v>26</v>
+      </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A113" s="4">
+      <c r="A113">
         <v>209</v>
       </c>
       <c r="B113" t="s">
@@ -6275,9 +5844,12 @@
       <c r="H113" t="s">
         <v>188</v>
       </c>
+      <c r="J113">
+        <v>21</v>
+      </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A114" s="4">
+      <c r="A114">
         <v>158</v>
       </c>
       <c r="B114" t="s">
@@ -6286,7 +5858,7 @@
       <c r="C114" t="s">
         <v>61</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="D114" s="7" t="s">
         <v>228</v>
       </c>
       <c r="E114" t="s">
@@ -6309,7 +5881,7 @@
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A115" s="4">
+      <c r="A115">
         <v>159</v>
       </c>
       <c r="B115" t="s">
@@ -6338,7 +5910,7 @@
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A116" s="4">
+      <c r="A116">
         <v>160</v>
       </c>
       <c r="B116" t="s">
@@ -6367,7 +5939,7 @@
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A117" s="4">
+      <c r="A117">
         <v>161</v>
       </c>
       <c r="B117" t="s">
@@ -6396,7 +5968,7 @@
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A118" s="4">
+      <c r="A118">
         <v>162</v>
       </c>
       <c r="B118" t="s">
@@ -6425,7 +5997,7 @@
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A119" s="4">
+      <c r="A119">
         <v>163</v>
       </c>
       <c r="B119" t="s">
@@ -6454,7 +6026,7 @@
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A120" s="4">
+      <c r="A120">
         <v>164</v>
       </c>
       <c r="B120" t="s">
@@ -6483,7 +6055,7 @@
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A121" s="4">
+      <c r="A121">
         <v>165</v>
       </c>
       <c r="B121" t="s">
@@ -6512,7 +6084,7 @@
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A122" s="4">
+      <c r="A122">
         <v>166</v>
       </c>
       <c r="B122" t="s">
@@ -6541,7 +6113,7 @@
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A123" s="4">
+      <c r="A123">
         <v>167</v>
       </c>
       <c r="B123" t="s">
@@ -6570,7 +6142,7 @@
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A124" s="4">
+      <c r="A124">
         <v>168</v>
       </c>
       <c r="B124" t="s">
@@ -6599,7 +6171,7 @@
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A125" s="4">
+      <c r="A125">
         <v>107</v>
       </c>
       <c r="B125" t="s">
@@ -6628,7 +6200,7 @@
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A126" s="4">
+      <c r="A126">
         <v>108</v>
       </c>
       <c r="B126" t="s">
@@ -6657,7 +6229,7 @@
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A127" s="4">
+      <c r="A127">
         <v>110</v>
       </c>
       <c r="B127" t="s">
@@ -6686,7 +6258,7 @@
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A128" s="4">
+      <c r="A128">
         <v>125</v>
       </c>
       <c r="B128" t="s">
@@ -6715,7 +6287,7 @@
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A129" s="4">
+      <c r="A129">
         <v>127</v>
       </c>
       <c r="B129" t="s">
@@ -6744,7 +6316,7 @@
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A130" s="4">
+      <c r="A130">
         <v>129</v>
       </c>
       <c r="B130" t="s">
@@ -6773,7 +6345,7 @@
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A131" s="4">
+      <c r="A131">
         <v>211</v>
       </c>
       <c r="B131" t="s">
@@ -6811,7 +6383,7 @@
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A132" s="4">
+      <c r="A132">
         <v>212</v>
       </c>
       <c r="B132" t="s">
@@ -6840,7 +6412,7 @@
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A133" s="4">
+      <c r="A133">
         <v>213</v>
       </c>
       <c r="B133" t="s">
@@ -6869,7 +6441,7 @@
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A134" s="4">
+      <c r="A134">
         <v>214</v>
       </c>
       <c r="B134" t="s">
@@ -6898,7 +6470,7 @@
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A135" s="4">
+      <c r="A135">
         <v>215</v>
       </c>
       <c r="B135" t="s">
@@ -6927,7 +6499,7 @@
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A136" s="4">
+      <c r="A136">
         <v>216</v>
       </c>
       <c r="B136" t="s">
@@ -6956,7 +6528,7 @@
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A137" s="4">
+      <c r="A137">
         <v>217</v>
       </c>
       <c r="B137" t="s">
@@ -6985,7 +6557,7 @@
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A138" s="4">
+      <c r="A138">
         <v>218</v>
       </c>
       <c r="B138" t="s">
@@ -7014,7 +6586,7 @@
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A139" s="4">
+      <c r="A139">
         <v>219</v>
       </c>
       <c r="B139" t="s">
@@ -7043,7 +6615,7 @@
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A140" s="4">
+      <c r="A140">
         <v>220</v>
       </c>
       <c r="B140" t="s">
@@ -7072,7 +6644,7 @@
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A141" s="4">
+      <c r="A141">
         <v>221</v>
       </c>
       <c r="B141" t="s">
@@ -7101,7 +6673,7 @@
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A142" s="4">
+      <c r="A142">
         <v>222</v>
       </c>
       <c r="B142" t="s">
@@ -7130,7 +6702,7 @@
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A143" s="4">
+      <c r="A143">
         <v>224</v>
       </c>
       <c r="B143" t="s">
@@ -7159,7 +6731,7 @@
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A144" s="4">
+      <c r="A144">
         <v>223</v>
       </c>
       <c r="B144" t="s">
@@ -7188,7 +6760,7 @@
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A145" s="4">
+      <c r="A145">
         <v>225</v>
       </c>
       <c r="B145" t="s">
@@ -7217,7 +6789,7 @@
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A146" s="4">
+      <c r="A146">
         <v>426</v>
       </c>
       <c r="B146" t="s">
@@ -7246,7 +6818,7 @@
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A147" s="4">
+      <c r="A147">
         <v>427</v>
       </c>
       <c r="B147" t="s">
@@ -7275,7 +6847,7 @@
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A148" s="4">
+      <c r="A148">
         <v>428</v>
       </c>
       <c r="B148" t="s">
@@ -7304,7 +6876,7 @@
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A149" s="4">
+      <c r="A149">
         <v>429</v>
       </c>
       <c r="B149" t="s">
@@ -7333,7 +6905,7 @@
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A150" s="4">
+      <c r="A150">
         <v>430</v>
       </c>
       <c r="B150" t="s">
@@ -7362,7 +6934,7 @@
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A151" s="4">
+      <c r="A151">
         <v>431</v>
       </c>
       <c r="B151" t="s">
@@ -7391,7 +6963,7 @@
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A152" s="4">
+      <c r="A152">
         <v>80</v>
       </c>
       <c r="B152" t="s">
@@ -7429,7 +7001,7 @@
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A153" s="4">
+      <c r="A153">
         <v>81</v>
       </c>
       <c r="B153" t="s">

</xml_diff>

<commit_message>
1005 sampling data entered
</commit_message>
<xml_diff>
--- a/F25_Sampling.xlsx
+++ b/F25_Sampling.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trini/Documents/Shedd/biota_project_genomicshifts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47085EA2-3DCE-5742-B98E-19B6D086D68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76102D90-512F-AA44-A928-D3940ABD96C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="1880" windowWidth="24040" windowHeight="12440" activeTab="1" xr2:uid="{07AAFEEF-A83C-484C-8992-E89847C75F27}"/>
+    <workbookView xWindow="860" yWindow="1020" windowWidth="24040" windowHeight="12440" activeTab="1" xr2:uid="{07AAFEEF-A83C-484C-8992-E89847C75F27}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$P$353</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="529">
   <si>
     <t xml:space="preserve">Bag </t>
   </si>
@@ -1267,6 +1270,363 @@
   </si>
   <si>
     <t>pic on phone for waypoint coordinates</t>
+  </si>
+  <si>
+    <t>F25_270</t>
+  </si>
+  <si>
+    <t>F25_272</t>
+  </si>
+  <si>
+    <t>F25_273</t>
+  </si>
+  <si>
+    <t>F25_274</t>
+  </si>
+  <si>
+    <t>F25_275</t>
+  </si>
+  <si>
+    <t>F25_277</t>
+  </si>
+  <si>
+    <t>F25_278</t>
+  </si>
+  <si>
+    <t>F25_279</t>
+  </si>
+  <si>
+    <t>10x3</t>
+  </si>
+  <si>
+    <t>6x3</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>F25_280</t>
+  </si>
+  <si>
+    <t>F25_281</t>
+  </si>
+  <si>
+    <t>F25_282</t>
+  </si>
+  <si>
+    <t>F25_254</t>
+  </si>
+  <si>
+    <t>F25_255</t>
+  </si>
+  <si>
+    <t>F25_256</t>
+  </si>
+  <si>
+    <t>F25_257</t>
+  </si>
+  <si>
+    <t>F25_258</t>
+  </si>
+  <si>
+    <t>1x.5</t>
+  </si>
+  <si>
+    <t>9x7</t>
+  </si>
+  <si>
+    <t>8x3</t>
+  </si>
+  <si>
+    <t>2.5x5</t>
+  </si>
+  <si>
+    <t>35x27</t>
+  </si>
+  <si>
+    <t>4.5x3</t>
+  </si>
+  <si>
+    <t>MCav</t>
+  </si>
+  <si>
+    <t>12x5</t>
+  </si>
+  <si>
+    <t>60x25</t>
+  </si>
+  <si>
+    <t>8x15</t>
+  </si>
+  <si>
+    <t>F25_301</t>
+  </si>
+  <si>
+    <t>F25_297</t>
+  </si>
+  <si>
+    <t>F25_299</t>
+  </si>
+  <si>
+    <t>F25_290</t>
+  </si>
+  <si>
+    <t>F25_286</t>
+  </si>
+  <si>
+    <t>F25_287</t>
+  </si>
+  <si>
+    <t>F25_285</t>
+  </si>
+  <si>
+    <t>F25_288</t>
+  </si>
+  <si>
+    <t>F25_300</t>
+  </si>
+  <si>
+    <t>F25_264</t>
+  </si>
+  <si>
+    <t>F25_298</t>
+  </si>
+  <si>
+    <t>F25_289</t>
+  </si>
+  <si>
+    <t>F25_295</t>
+  </si>
+  <si>
+    <t>F25_294</t>
+  </si>
+  <si>
+    <t>F25_291</t>
+  </si>
+  <si>
+    <t>F25_292</t>
+  </si>
+  <si>
+    <t>F25_293</t>
+  </si>
+  <si>
+    <t>F25_302</t>
+  </si>
+  <si>
+    <t>F25_284</t>
+  </si>
+  <si>
+    <t>F25_263</t>
+  </si>
+  <si>
+    <t>F25_268</t>
+  </si>
+  <si>
+    <t>F25_283</t>
+  </si>
+  <si>
+    <t>F25_269</t>
+  </si>
+  <si>
+    <t>F25_266</t>
+  </si>
+  <si>
+    <t>F25_259</t>
+  </si>
+  <si>
+    <t>F25_267</t>
+  </si>
+  <si>
+    <t>F25_260</t>
+  </si>
+  <si>
+    <t>F25_261</t>
+  </si>
+  <si>
+    <t>F25_262</t>
+  </si>
+  <si>
+    <t>25x5</t>
+  </si>
+  <si>
+    <t>20x9</t>
+  </si>
+  <si>
+    <t>25x17</t>
+  </si>
+  <si>
+    <t>7x1</t>
+  </si>
+  <si>
+    <t>blank_1</t>
+  </si>
+  <si>
+    <t>F25_336</t>
+  </si>
+  <si>
+    <t>F25_335</t>
+  </si>
+  <si>
+    <t>F25_324</t>
+  </si>
+  <si>
+    <t>F25_318</t>
+  </si>
+  <si>
+    <t>F25_321</t>
+  </si>
+  <si>
+    <t>F25_333</t>
+  </si>
+  <si>
+    <t>F25_319</t>
+  </si>
+  <si>
+    <t>F25_317</t>
+  </si>
+  <si>
+    <t>F25_334</t>
+  </si>
+  <si>
+    <t>F25_330</t>
+  </si>
+  <si>
+    <t>F25_325</t>
+  </si>
+  <si>
+    <t>F25_328</t>
+  </si>
+  <si>
+    <t>F25_331</t>
+  </si>
+  <si>
+    <t>F25_332</t>
+  </si>
+  <si>
+    <t>F25_326</t>
+  </si>
+  <si>
+    <t>F25_327</t>
+  </si>
+  <si>
+    <t>F25_320</t>
+  </si>
+  <si>
+    <t>F25_329</t>
+  </si>
+  <si>
+    <t>F25_323</t>
+  </si>
+  <si>
+    <t>F25_316</t>
+  </si>
+  <si>
+    <t>F25_311</t>
+  </si>
+  <si>
+    <t>F25_315</t>
+  </si>
+  <si>
+    <t>F25_308</t>
+  </si>
+  <si>
+    <t>F25_310</t>
+  </si>
+  <si>
+    <t>F25_309</t>
+  </si>
+  <si>
+    <t>F25_305</t>
+  </si>
+  <si>
+    <t>F25_314</t>
+  </si>
+  <si>
+    <t>F25_306</t>
+  </si>
+  <si>
+    <t>F25_313</t>
+  </si>
+  <si>
+    <t>F25_304</t>
+  </si>
+  <si>
+    <t>F25_303</t>
+  </si>
+  <si>
+    <t>F25_307</t>
+  </si>
+  <si>
+    <t>70x80</t>
+  </si>
+  <si>
+    <t>7x8</t>
+  </si>
+  <si>
+    <t>6x7</t>
+  </si>
+  <si>
+    <t>2x3</t>
+  </si>
+  <si>
+    <t>6x4</t>
+  </si>
+  <si>
+    <t>4x5</t>
+  </si>
+  <si>
+    <t>10x20</t>
+  </si>
+  <si>
+    <t>F25_342</t>
+  </si>
+  <si>
+    <t>F25_340</t>
+  </si>
+  <si>
+    <t>F25_338</t>
+  </si>
+  <si>
+    <t>F25_337</t>
+  </si>
+  <si>
+    <t>F25_350</t>
+  </si>
+  <si>
+    <t>F25_339</t>
+  </si>
+  <si>
+    <t>F25_345</t>
+  </si>
+  <si>
+    <t>F25_341</t>
+  </si>
+  <si>
+    <t>F25_344</t>
+  </si>
+  <si>
+    <t>F25_343</t>
+  </si>
+  <si>
+    <t>F25_346</t>
+  </si>
+  <si>
+    <t>F25_348</t>
+  </si>
+  <si>
+    <t>F25_347</t>
+  </si>
+  <si>
+    <t>F25_349</t>
+  </si>
+  <si>
+    <t>1x2</t>
+  </si>
+  <si>
+    <t>11x6</t>
+  </si>
+  <si>
+    <t>3x4</t>
   </si>
 </sst>
 </file>
@@ -2429,10 +2789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859618DA-7D2E-F14A-9531-A0F7323C3157}">
-  <dimension ref="A1:P257"/>
+  <dimension ref="A1:P353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J114" sqref="J114"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="F354" sqref="F354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2585,15 +2945,15 @@
       </c>
       <c r="N4" s="20">
         <f>COUNTIFS(C:C, "Cnat")</f>
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="O4" s="12">
         <f>COUNTIFS(C:C,"Cnat", F:F, "Y" )</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="P4" s="17">
         <f>COUNTIFS(C:C,"Cnat", F:F, "N" )</f>
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2632,15 +2992,15 @@
       </c>
       <c r="N5" s="21">
         <f>COUNTIFS(C:C, "Dlab")</f>
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="O5" s="13">
         <f>COUNTIFS(C:C,"Dlab", F:F, "Y" )</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P5" s="18">
         <f>COUNTIFS(C:C,"Dlab", F:F, "N" )</f>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -2676,15 +3036,15 @@
       </c>
       <c r="N6" s="21">
         <f>COUNTIFS(C:C,"Mcav")</f>
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="O6" s="13">
         <f>COUNTIFS(C:C,"Mcav", F:F, "Y" )</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="P6" s="18">
         <f>COUNTIFS(C:C,"Mcav", F:F, "N" )</f>
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -2720,15 +3080,15 @@
       </c>
       <c r="N7" s="21">
         <f>COUNTIFS(C:C, "Sint")</f>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="O7" s="14">
         <f>COUNTIFS(C:C,"Sint", F:F, "Y" )</f>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="P7" s="18">
         <f>COUNTIFS(C:C,"Sint", F:F, "N" )</f>
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -2767,15 +3127,15 @@
       </c>
       <c r="N8" s="21">
         <f>COUNTIFS(C:C, "Past")</f>
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="O8" s="13">
         <f>COUNTIFS(C:C,"Past", F:F, "Y" )</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="P8" s="18">
         <f>COUNTIFS(C:C,"Past", F:F, "N" )</f>
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -2814,15 +3174,15 @@
       </c>
       <c r="N9" s="21">
         <f>COUNTIFS(C:C, "Pstr")</f>
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="O9" s="13">
         <f>COUNTIFS(C:C,"Pstr", F:F, "Y" )</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="P9" s="18">
         <f>COUNTIFS(C:C,"Pstr", F:F, "N" )</f>
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -2858,15 +3218,15 @@
       </c>
       <c r="N10" s="21">
         <f>COUNTIFS(C:C, "Ssid")</f>
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="O10" s="13">
         <f>COUNTIFS(C:C,"Ssid", F:F, "Y" )</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="P10" s="18">
         <f>COUNTIFS(C:C,"Ssid", F:F, "N" )</f>
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2900,7 +3260,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="6">
         <f>SUM(N4:N10)</f>
-        <v>252</v>
+        <v>347</v>
       </c>
       <c r="O11" s="15"/>
       <c r="P11" s="19"/>
@@ -9994,7 +10354,2783 @@
         <v>20</v>
       </c>
     </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>432</v>
+      </c>
+      <c r="B258" t="s">
+        <v>410</v>
+      </c>
+      <c r="C258" t="s">
+        <v>59</v>
+      </c>
+      <c r="D258">
+        <v>314</v>
+      </c>
+      <c r="E258" t="s">
+        <v>418</v>
+      </c>
+      <c r="F258" t="s">
+        <v>66</v>
+      </c>
+      <c r="G258">
+        <v>20251005</v>
+      </c>
+      <c r="H258" t="s">
+        <v>19</v>
+      </c>
+      <c r="J258">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>433</v>
+      </c>
+      <c r="B259" t="s">
+        <v>411</v>
+      </c>
+      <c r="C259" t="s">
+        <v>61</v>
+      </c>
+      <c r="D259">
+        <v>314</v>
+      </c>
+      <c r="E259" t="s">
+        <v>306</v>
+      </c>
+      <c r="F259" t="s">
+        <v>66</v>
+      </c>
+      <c r="G259">
+        <v>20251005</v>
+      </c>
+      <c r="H259" t="s">
+        <v>19</v>
+      </c>
+      <c r="J259">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>434</v>
+      </c>
+      <c r="B260" t="s">
+        <v>412</v>
+      </c>
+      <c r="C260" t="s">
+        <v>60</v>
+      </c>
+      <c r="D260">
+        <v>314</v>
+      </c>
+      <c r="E260" t="s">
+        <v>419</v>
+      </c>
+      <c r="F260" t="s">
+        <v>66</v>
+      </c>
+      <c r="G260">
+        <v>20251005</v>
+      </c>
+      <c r="H260" t="s">
+        <v>19</v>
+      </c>
+      <c r="J260">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>435</v>
+      </c>
+      <c r="B261" t="s">
+        <v>413</v>
+      </c>
+      <c r="C261" t="s">
+        <v>62</v>
+      </c>
+      <c r="D261">
+        <v>314</v>
+      </c>
+      <c r="E261" t="s">
+        <v>86</v>
+      </c>
+      <c r="F261" t="s">
+        <v>67</v>
+      </c>
+      <c r="G261">
+        <v>20251005</v>
+      </c>
+      <c r="H261" t="s">
+        <v>19</v>
+      </c>
+      <c r="J261">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>436</v>
+      </c>
+      <c r="B262" t="s">
+        <v>414</v>
+      </c>
+      <c r="C262" t="s">
+        <v>63</v>
+      </c>
+      <c r="D262">
+        <v>314</v>
+      </c>
+      <c r="E262" t="s">
+        <v>83</v>
+      </c>
+      <c r="F262" t="s">
+        <v>67</v>
+      </c>
+      <c r="G262">
+        <v>20251005</v>
+      </c>
+      <c r="H262" t="s">
+        <v>19</v>
+      </c>
+      <c r="J262">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>437</v>
+      </c>
+      <c r="B263" t="s">
+        <v>414</v>
+      </c>
+      <c r="C263" t="s">
+        <v>61</v>
+      </c>
+      <c r="D263">
+        <v>314</v>
+      </c>
+      <c r="E263" t="s">
+        <v>135</v>
+      </c>
+      <c r="F263" t="s">
+        <v>67</v>
+      </c>
+      <c r="G263">
+        <v>20251005</v>
+      </c>
+      <c r="H263" t="s">
+        <v>19</v>
+      </c>
+      <c r="J263">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>438</v>
+      </c>
+      <c r="B264" t="s">
+        <v>415</v>
+      </c>
+      <c r="C264" t="s">
+        <v>63</v>
+      </c>
+      <c r="D264">
+        <v>314</v>
+      </c>
+      <c r="E264" t="s">
+        <v>83</v>
+      </c>
+      <c r="F264" t="s">
+        <v>67</v>
+      </c>
+      <c r="G264">
+        <v>20251005</v>
+      </c>
+      <c r="H264" t="s">
+        <v>19</v>
+      </c>
+      <c r="J264">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>439</v>
+      </c>
+      <c r="B265" t="s">
+        <v>416</v>
+      </c>
+      <c r="C265" t="s">
+        <v>60</v>
+      </c>
+      <c r="D265">
+        <v>314</v>
+      </c>
+      <c r="E265" t="s">
+        <v>137</v>
+      </c>
+      <c r="F265" t="s">
+        <v>66</v>
+      </c>
+      <c r="G265">
+        <v>20251005</v>
+      </c>
+      <c r="H265" t="s">
+        <v>19</v>
+      </c>
+      <c r="J265">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>440</v>
+      </c>
+      <c r="B266" t="s">
+        <v>417</v>
+      </c>
+      <c r="C266" t="s">
+        <v>63</v>
+      </c>
+      <c r="D266">
+        <v>314</v>
+      </c>
+      <c r="E266" t="s">
+        <v>399</v>
+      </c>
+      <c r="F266" t="s">
+        <v>66</v>
+      </c>
+      <c r="G266">
+        <v>20251005</v>
+      </c>
+      <c r="H266" t="s">
+        <v>19</v>
+      </c>
+      <c r="J266">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>300</v>
+      </c>
+      <c r="B267" t="s">
+        <v>421</v>
+      </c>
+      <c r="C267" t="s">
+        <v>59</v>
+      </c>
+      <c r="D267">
+        <v>1475</v>
+      </c>
+      <c r="E267" t="s">
+        <v>140</v>
+      </c>
+      <c r="F267" t="s">
+        <v>67</v>
+      </c>
+      <c r="G267">
+        <v>20251005</v>
+      </c>
+      <c r="H267" t="s">
+        <v>420</v>
+      </c>
+      <c r="J267">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>299</v>
+      </c>
+      <c r="B268" t="s">
+        <v>422</v>
+      </c>
+      <c r="C268" t="s">
+        <v>61</v>
+      </c>
+      <c r="D268">
+        <v>1475</v>
+      </c>
+      <c r="E268" t="s">
+        <v>429</v>
+      </c>
+      <c r="F268" t="s">
+        <v>67</v>
+      </c>
+      <c r="G268">
+        <v>20251005</v>
+      </c>
+      <c r="H268" t="s">
+        <v>420</v>
+      </c>
+      <c r="J268">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>298</v>
+      </c>
+      <c r="B269" t="s">
+        <v>423</v>
+      </c>
+      <c r="C269" t="s">
+        <v>61</v>
+      </c>
+      <c r="D269">
+        <v>1475</v>
+      </c>
+      <c r="E269" t="s">
+        <v>405</v>
+      </c>
+      <c r="F269" t="s">
+        <v>66</v>
+      </c>
+      <c r="G269">
+        <v>20251005</v>
+      </c>
+      <c r="H269" t="s">
+        <v>420</v>
+      </c>
+      <c r="J269">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>297</v>
+      </c>
+      <c r="B270" t="s">
+        <v>424</v>
+      </c>
+      <c r="C270" t="s">
+        <v>59</v>
+      </c>
+      <c r="D270">
+        <v>1475</v>
+      </c>
+      <c r="E270" t="s">
+        <v>430</v>
+      </c>
+      <c r="F270" t="s">
+        <v>66</v>
+      </c>
+      <c r="G270">
+        <v>20251005</v>
+      </c>
+      <c r="H270" t="s">
+        <v>420</v>
+      </c>
+      <c r="J270">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>296</v>
+      </c>
+      <c r="B271" t="s">
+        <v>425</v>
+      </c>
+      <c r="C271" t="s">
+        <v>62</v>
+      </c>
+      <c r="D271">
+        <v>1475</v>
+      </c>
+      <c r="E271" t="s">
+        <v>431</v>
+      </c>
+      <c r="F271" t="s">
+        <v>66</v>
+      </c>
+      <c r="G271">
+        <v>20251005</v>
+      </c>
+      <c r="H271" t="s">
+        <v>420</v>
+      </c>
+      <c r="J271">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>295</v>
+      </c>
+      <c r="B272" t="s">
+        <v>426</v>
+      </c>
+      <c r="C272" t="s">
+        <v>62</v>
+      </c>
+      <c r="D272">
+        <v>1475</v>
+      </c>
+      <c r="E272" t="s">
+        <v>432</v>
+      </c>
+      <c r="F272" t="s">
+        <v>67</v>
+      </c>
+      <c r="G272">
+        <v>20251005</v>
+      </c>
+      <c r="H272" t="s">
+        <v>420</v>
+      </c>
+      <c r="J272">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>293</v>
+      </c>
+      <c r="B273" t="s">
+        <v>427</v>
+      </c>
+      <c r="C273" t="s">
+        <v>60</v>
+      </c>
+      <c r="D273">
+        <v>1475</v>
+      </c>
+      <c r="E273" t="s">
+        <v>433</v>
+      </c>
+      <c r="F273" t="s">
+        <v>66</v>
+      </c>
+      <c r="G273">
+        <v>20251005</v>
+      </c>
+      <c r="H273" t="s">
+        <v>420</v>
+      </c>
+      <c r="J273">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>292</v>
+      </c>
+      <c r="B274" t="s">
+        <v>428</v>
+      </c>
+      <c r="C274" t="s">
+        <v>63</v>
+      </c>
+      <c r="D274">
+        <v>1475</v>
+      </c>
+      <c r="E274" t="s">
+        <v>434</v>
+      </c>
+      <c r="F274" t="s">
+        <v>67</v>
+      </c>
+      <c r="G274">
+        <v>20251005</v>
+      </c>
+      <c r="H274" t="s">
+        <v>420</v>
+      </c>
+      <c r="J274">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>326</v>
+      </c>
+      <c r="B275" t="s">
+        <v>439</v>
+      </c>
+      <c r="C275" t="s">
+        <v>63</v>
+      </c>
+      <c r="D275">
+        <v>2465</v>
+      </c>
+      <c r="E275" t="s">
+        <v>230</v>
+      </c>
+      <c r="F275" t="s">
+        <v>66</v>
+      </c>
+      <c r="G275">
+        <v>20251005</v>
+      </c>
+      <c r="H275" t="s">
+        <v>18</v>
+      </c>
+      <c r="J275">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>327</v>
+      </c>
+      <c r="B276" t="s">
+        <v>440</v>
+      </c>
+      <c r="C276" t="s">
+        <v>61</v>
+      </c>
+      <c r="D276">
+        <v>2465</v>
+      </c>
+      <c r="E276" t="s">
+        <v>86</v>
+      </c>
+      <c r="F276" t="s">
+        <v>67</v>
+      </c>
+      <c r="G276">
+        <v>20251005</v>
+      </c>
+      <c r="H276" t="s">
+        <v>18</v>
+      </c>
+      <c r="J276">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>328</v>
+      </c>
+      <c r="B277" t="s">
+        <v>441</v>
+      </c>
+      <c r="C277" t="s">
+        <v>62</v>
+      </c>
+      <c r="D277">
+        <v>2465</v>
+      </c>
+      <c r="E277" t="s">
+        <v>86</v>
+      </c>
+      <c r="F277" t="s">
+        <v>67</v>
+      </c>
+      <c r="G277">
+        <v>20251005</v>
+      </c>
+      <c r="H277" t="s">
+        <v>18</v>
+      </c>
+      <c r="J277">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>329</v>
+      </c>
+      <c r="B278" t="s">
+        <v>442</v>
+      </c>
+      <c r="C278" t="s">
+        <v>435</v>
+      </c>
+      <c r="D278">
+        <v>2465</v>
+      </c>
+      <c r="E278" t="s">
+        <v>431</v>
+      </c>
+      <c r="F278" t="s">
+        <v>66</v>
+      </c>
+      <c r="G278">
+        <v>20251005</v>
+      </c>
+      <c r="H278" t="s">
+        <v>18</v>
+      </c>
+      <c r="J278">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>330</v>
+      </c>
+      <c r="B279" t="s">
+        <v>443</v>
+      </c>
+      <c r="C279" t="s">
+        <v>62</v>
+      </c>
+      <c r="D279">
+        <v>2465</v>
+      </c>
+      <c r="E279" t="s">
+        <v>436</v>
+      </c>
+      <c r="F279" t="s">
+        <v>66</v>
+      </c>
+      <c r="G279">
+        <v>20251005</v>
+      </c>
+      <c r="H279" t="s">
+        <v>18</v>
+      </c>
+      <c r="J279">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>331</v>
+      </c>
+      <c r="B280" t="s">
+        <v>444</v>
+      </c>
+      <c r="C280" t="s">
+        <v>61</v>
+      </c>
+      <c r="D280">
+        <v>2465</v>
+      </c>
+      <c r="E280" t="s">
+        <v>437</v>
+      </c>
+      <c r="F280" t="s">
+        <v>66</v>
+      </c>
+      <c r="G280">
+        <v>20251005</v>
+      </c>
+      <c r="H280" t="s">
+        <v>18</v>
+      </c>
+      <c r="J280">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>332</v>
+      </c>
+      <c r="B281" t="s">
+        <v>445</v>
+      </c>
+      <c r="C281" t="s">
+        <v>64</v>
+      </c>
+      <c r="D281">
+        <v>2465</v>
+      </c>
+      <c r="E281" t="s">
+        <v>400</v>
+      </c>
+      <c r="F281" t="s">
+        <v>66</v>
+      </c>
+      <c r="G281">
+        <v>20251005</v>
+      </c>
+      <c r="H281" t="s">
+        <v>18</v>
+      </c>
+      <c r="J281">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>333</v>
+      </c>
+      <c r="B282" t="s">
+        <v>446</v>
+      </c>
+      <c r="C282" t="s">
+        <v>60</v>
+      </c>
+      <c r="D282">
+        <v>2465</v>
+      </c>
+      <c r="E282" t="s">
+        <v>80</v>
+      </c>
+      <c r="F282" t="s">
+        <v>67</v>
+      </c>
+      <c r="G282">
+        <v>20251005</v>
+      </c>
+      <c r="H282" t="s">
+        <v>18</v>
+      </c>
+      <c r="J282">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>334</v>
+      </c>
+      <c r="B283" t="s">
+        <v>447</v>
+      </c>
+      <c r="C283" t="s">
+        <v>63</v>
+      </c>
+      <c r="D283">
+        <v>2465</v>
+      </c>
+      <c r="E283" t="s">
+        <v>419</v>
+      </c>
+      <c r="F283" t="s">
+        <v>66</v>
+      </c>
+      <c r="G283">
+        <v>20251005</v>
+      </c>
+      <c r="H283" t="s">
+        <v>18</v>
+      </c>
+      <c r="J283">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>335</v>
+      </c>
+      <c r="B284" t="s">
+        <v>448</v>
+      </c>
+      <c r="C284" t="s">
+        <v>59</v>
+      </c>
+      <c r="D284">
+        <v>2465</v>
+      </c>
+      <c r="E284" t="s">
+        <v>438</v>
+      </c>
+      <c r="F284" t="s">
+        <v>66</v>
+      </c>
+      <c r="G284">
+        <v>20251005</v>
+      </c>
+      <c r="H284" t="s">
+        <v>18</v>
+      </c>
+      <c r="J284">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>336</v>
+      </c>
+      <c r="B285" t="s">
+        <v>449</v>
+      </c>
+      <c r="C285" t="s">
+        <v>63</v>
+      </c>
+      <c r="D285">
+        <v>2465</v>
+      </c>
+      <c r="E285" t="s">
+        <v>357</v>
+      </c>
+      <c r="F285" t="s">
+        <v>66</v>
+      </c>
+      <c r="G285">
+        <v>20251005</v>
+      </c>
+      <c r="H285" t="s">
+        <v>18</v>
+      </c>
+      <c r="J285">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>337</v>
+      </c>
+      <c r="B286" t="s">
+        <v>450</v>
+      </c>
+      <c r="C286" t="s">
+        <v>64</v>
+      </c>
+      <c r="D286">
+        <v>2465</v>
+      </c>
+      <c r="E286" t="s">
+        <v>351</v>
+      </c>
+      <c r="F286" t="s">
+        <v>66</v>
+      </c>
+      <c r="G286">
+        <v>20251005</v>
+      </c>
+      <c r="H286" t="s">
+        <v>18</v>
+      </c>
+      <c r="J286">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>338</v>
+      </c>
+      <c r="B287" t="s">
+        <v>451</v>
+      </c>
+      <c r="C287" t="s">
+        <v>65</v>
+      </c>
+      <c r="D287">
+        <v>2465</v>
+      </c>
+      <c r="E287">
+        <v>205</v>
+      </c>
+      <c r="F287" t="s">
+        <v>66</v>
+      </c>
+      <c r="G287">
+        <v>20251005</v>
+      </c>
+      <c r="H287" t="s">
+        <v>18</v>
+      </c>
+      <c r="J287">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>339</v>
+      </c>
+      <c r="B288" t="s">
+        <v>452</v>
+      </c>
+      <c r="C288" t="s">
+        <v>59</v>
+      </c>
+      <c r="D288">
+        <v>2465</v>
+      </c>
+      <c r="E288" t="s">
+        <v>86</v>
+      </c>
+      <c r="F288" t="s">
+        <v>67</v>
+      </c>
+      <c r="G288">
+        <v>20251005</v>
+      </c>
+      <c r="H288" t="s">
+        <v>18</v>
+      </c>
+      <c r="J288">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>340</v>
+      </c>
+      <c r="B289" t="s">
+        <v>453</v>
+      </c>
+      <c r="C289" t="s">
+        <v>64</v>
+      </c>
+      <c r="D289">
+        <v>2465</v>
+      </c>
+      <c r="E289" t="s">
+        <v>84</v>
+      </c>
+      <c r="F289" t="s">
+        <v>67</v>
+      </c>
+      <c r="G289">
+        <v>20251005</v>
+      </c>
+      <c r="H289" t="s">
+        <v>18</v>
+      </c>
+      <c r="J289">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>341</v>
+      </c>
+      <c r="B290" t="s">
+        <v>454</v>
+      </c>
+      <c r="C290" t="s">
+        <v>63</v>
+      </c>
+      <c r="D290">
+        <v>2462</v>
+      </c>
+      <c r="E290" t="s">
+        <v>144</v>
+      </c>
+      <c r="F290" t="s">
+        <v>66</v>
+      </c>
+      <c r="G290">
+        <v>20251005</v>
+      </c>
+      <c r="H290" t="s">
+        <v>18</v>
+      </c>
+      <c r="J290">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>342</v>
+      </c>
+      <c r="B291" t="s">
+        <v>452</v>
+      </c>
+      <c r="C291" t="s">
+        <v>62</v>
+      </c>
+      <c r="D291">
+        <v>2462</v>
+      </c>
+      <c r="E291" t="s">
+        <v>84</v>
+      </c>
+      <c r="F291" t="s">
+        <v>67</v>
+      </c>
+      <c r="G291">
+        <v>20251005</v>
+      </c>
+      <c r="H291" t="s">
+        <v>18</v>
+      </c>
+      <c r="J291">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>343</v>
+      </c>
+      <c r="B292" t="s">
+        <v>455</v>
+      </c>
+      <c r="C292" t="s">
+        <v>61</v>
+      </c>
+      <c r="D292">
+        <v>2462</v>
+      </c>
+      <c r="E292" t="s">
+        <v>468</v>
+      </c>
+      <c r="F292" t="s">
+        <v>66</v>
+      </c>
+      <c r="G292">
+        <v>20251005</v>
+      </c>
+      <c r="H292" t="s">
+        <v>18</v>
+      </c>
+      <c r="J292">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>344</v>
+      </c>
+      <c r="B293" t="s">
+        <v>456</v>
+      </c>
+      <c r="C293" t="s">
+        <v>60</v>
+      </c>
+      <c r="D293">
+        <v>2462</v>
+      </c>
+      <c r="E293" t="s">
+        <v>144</v>
+      </c>
+      <c r="F293" t="s">
+        <v>66</v>
+      </c>
+      <c r="G293">
+        <v>20251005</v>
+      </c>
+      <c r="H293" t="s">
+        <v>18</v>
+      </c>
+      <c r="J293">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>345</v>
+      </c>
+      <c r="B294" t="s">
+        <v>445</v>
+      </c>
+      <c r="C294" t="s">
+        <v>59</v>
+      </c>
+      <c r="D294">
+        <v>2462</v>
+      </c>
+      <c r="E294" t="s">
+        <v>84</v>
+      </c>
+      <c r="F294" t="s">
+        <v>67</v>
+      </c>
+      <c r="G294">
+        <v>20251005</v>
+      </c>
+      <c r="H294" t="s">
+        <v>18</v>
+      </c>
+      <c r="J294">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>346</v>
+      </c>
+      <c r="B295" t="s">
+        <v>457</v>
+      </c>
+      <c r="C295" t="s">
+        <v>60</v>
+      </c>
+      <c r="D295">
+        <v>2462</v>
+      </c>
+      <c r="E295" t="s">
+        <v>86</v>
+      </c>
+      <c r="F295" t="s">
+        <v>67</v>
+      </c>
+      <c r="G295">
+        <v>20251005</v>
+      </c>
+      <c r="H295" t="s">
+        <v>18</v>
+      </c>
+      <c r="J295">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>347</v>
+      </c>
+      <c r="B296" t="s">
+        <v>458</v>
+      </c>
+      <c r="C296" t="s">
+        <v>65</v>
+      </c>
+      <c r="D296">
+        <v>2462</v>
+      </c>
+      <c r="E296" t="s">
+        <v>84</v>
+      </c>
+      <c r="F296" t="s">
+        <v>67</v>
+      </c>
+      <c r="G296">
+        <v>20251005</v>
+      </c>
+      <c r="H296" t="s">
+        <v>18</v>
+      </c>
+      <c r="J296">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>348</v>
+      </c>
+      <c r="B297" t="s">
+        <v>459</v>
+      </c>
+      <c r="C297" t="s">
+        <v>59</v>
+      </c>
+      <c r="D297">
+        <v>2462</v>
+      </c>
+      <c r="E297" t="s">
+        <v>438</v>
+      </c>
+      <c r="F297" t="s">
+        <v>66</v>
+      </c>
+      <c r="G297">
+        <v>20251005</v>
+      </c>
+      <c r="H297" t="s">
+        <v>18</v>
+      </c>
+      <c r="J297">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>349</v>
+      </c>
+      <c r="B298" t="s">
+        <v>460</v>
+      </c>
+      <c r="C298" t="s">
+        <v>63</v>
+      </c>
+      <c r="D298">
+        <v>2462</v>
+      </c>
+      <c r="E298" t="s">
+        <v>469</v>
+      </c>
+      <c r="F298" t="s">
+        <v>66</v>
+      </c>
+      <c r="G298">
+        <v>20251005</v>
+      </c>
+      <c r="H298" t="s">
+        <v>18</v>
+      </c>
+      <c r="J298">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>350</v>
+      </c>
+      <c r="B299" t="s">
+        <v>461</v>
+      </c>
+      <c r="C299" t="s">
+        <v>64</v>
+      </c>
+      <c r="D299">
+        <v>2462</v>
+      </c>
+      <c r="E299" t="s">
+        <v>203</v>
+      </c>
+      <c r="F299" t="s">
+        <v>66</v>
+      </c>
+      <c r="G299">
+        <v>20251005</v>
+      </c>
+      <c r="H299" t="s">
+        <v>18</v>
+      </c>
+      <c r="J299">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>351</v>
+      </c>
+      <c r="B300" t="s">
+        <v>462</v>
+      </c>
+      <c r="C300" t="s">
+        <v>62</v>
+      </c>
+      <c r="D300">
+        <v>2462</v>
+      </c>
+      <c r="E300" t="s">
+        <v>470</v>
+      </c>
+      <c r="F300" t="s">
+        <v>66</v>
+      </c>
+      <c r="G300">
+        <v>20251005</v>
+      </c>
+      <c r="H300" t="s">
+        <v>18</v>
+      </c>
+      <c r="J300">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>352</v>
+      </c>
+      <c r="B301" t="s">
+        <v>463</v>
+      </c>
+      <c r="C301" t="s">
+        <v>65</v>
+      </c>
+      <c r="D301">
+        <v>2462</v>
+      </c>
+      <c r="E301" t="s">
+        <v>87</v>
+      </c>
+      <c r="F301" t="s">
+        <v>66</v>
+      </c>
+      <c r="G301">
+        <v>20251005</v>
+      </c>
+      <c r="H301" t="s">
+        <v>18</v>
+      </c>
+      <c r="J301">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>353</v>
+      </c>
+      <c r="B302" t="s">
+        <v>464</v>
+      </c>
+      <c r="C302" t="s">
+        <v>64</v>
+      </c>
+      <c r="D302">
+        <v>2462</v>
+      </c>
+      <c r="E302" t="s">
+        <v>80</v>
+      </c>
+      <c r="F302" t="s">
+        <v>67</v>
+      </c>
+      <c r="G302">
+        <v>20251005</v>
+      </c>
+      <c r="H302" t="s">
+        <v>18</v>
+      </c>
+      <c r="J302">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>354</v>
+      </c>
+      <c r="B303" t="s">
+        <v>465</v>
+      </c>
+      <c r="C303" t="s">
+        <v>61</v>
+      </c>
+      <c r="D303">
+        <v>2462</v>
+      </c>
+      <c r="E303" t="s">
+        <v>86</v>
+      </c>
+      <c r="F303" t="s">
+        <v>67</v>
+      </c>
+      <c r="G303">
+        <v>20251005</v>
+      </c>
+      <c r="H303" t="s">
+        <v>18</v>
+      </c>
+      <c r="J303">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>355</v>
+      </c>
+      <c r="B304" t="s">
+        <v>466</v>
+      </c>
+      <c r="C304" t="s">
+        <v>65</v>
+      </c>
+      <c r="D304">
+        <v>2462</v>
+      </c>
+      <c r="E304" t="s">
+        <v>83</v>
+      </c>
+      <c r="F304" t="s">
+        <v>66</v>
+      </c>
+      <c r="G304">
+        <v>20251005</v>
+      </c>
+      <c r="H304" t="s">
+        <v>18</v>
+      </c>
+      <c r="J304">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>356</v>
+      </c>
+      <c r="B305" t="s">
+        <v>467</v>
+      </c>
+      <c r="C305" t="s">
+        <v>63</v>
+      </c>
+      <c r="D305">
+        <v>2462</v>
+      </c>
+      <c r="E305" t="s">
+        <v>471</v>
+      </c>
+      <c r="F305" t="s">
+        <v>66</v>
+      </c>
+      <c r="G305">
+        <v>20251005</v>
+      </c>
+      <c r="H305" t="s">
+        <v>18</v>
+      </c>
+      <c r="J305">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>382</v>
+      </c>
+      <c r="B306" t="s">
+        <v>473</v>
+      </c>
+      <c r="C306" t="s">
+        <v>65</v>
+      </c>
+      <c r="D306">
+        <v>2491</v>
+      </c>
+      <c r="E306" t="s">
+        <v>395</v>
+      </c>
+      <c r="F306" t="s">
+        <v>67</v>
+      </c>
+      <c r="G306">
+        <v>20251005</v>
+      </c>
+      <c r="H306" t="s">
+        <v>17</v>
+      </c>
+      <c r="J306">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>408</v>
+      </c>
+      <c r="B307" t="s">
+        <v>474</v>
+      </c>
+      <c r="C307" t="s">
+        <v>61</v>
+      </c>
+      <c r="D307">
+        <v>2491</v>
+      </c>
+      <c r="E307" t="s">
+        <v>505</v>
+      </c>
+      <c r="F307" t="s">
+        <v>66</v>
+      </c>
+      <c r="G307">
+        <v>20251005</v>
+      </c>
+      <c r="H307" t="s">
+        <v>17</v>
+      </c>
+      <c r="J307">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>409</v>
+      </c>
+      <c r="B308" t="s">
+        <v>475</v>
+      </c>
+      <c r="C308" t="s">
+        <v>63</v>
+      </c>
+      <c r="D308">
+        <v>2491</v>
+      </c>
+      <c r="E308" t="s">
+        <v>506</v>
+      </c>
+      <c r="F308" t="s">
+        <v>66</v>
+      </c>
+      <c r="G308">
+        <v>20251005</v>
+      </c>
+      <c r="H308" t="s">
+        <v>17</v>
+      </c>
+      <c r="J308">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>410</v>
+      </c>
+      <c r="B309" t="s">
+        <v>476</v>
+      </c>
+      <c r="C309" t="s">
+        <v>65</v>
+      </c>
+      <c r="D309">
+        <v>2491</v>
+      </c>
+      <c r="E309" t="s">
+        <v>200</v>
+      </c>
+      <c r="F309" t="s">
+        <v>66</v>
+      </c>
+      <c r="G309">
+        <v>20251005</v>
+      </c>
+      <c r="H309" t="s">
+        <v>17</v>
+      </c>
+      <c r="J309">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>411</v>
+      </c>
+      <c r="B310" t="s">
+        <v>477</v>
+      </c>
+      <c r="C310" t="s">
+        <v>59</v>
+      </c>
+      <c r="D310">
+        <v>2491</v>
+      </c>
+      <c r="E310" t="s">
+        <v>318</v>
+      </c>
+      <c r="F310" t="s">
+        <v>66</v>
+      </c>
+      <c r="G310">
+        <v>20251005</v>
+      </c>
+      <c r="H310" t="s">
+        <v>17</v>
+      </c>
+      <c r="J310">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>413</v>
+      </c>
+      <c r="B311" t="s">
+        <v>478</v>
+      </c>
+      <c r="C311" t="s">
+        <v>60</v>
+      </c>
+      <c r="D311">
+        <v>2491</v>
+      </c>
+      <c r="E311" t="s">
+        <v>24</v>
+      </c>
+      <c r="F311" t="s">
+        <v>66</v>
+      </c>
+      <c r="G311">
+        <v>20251005</v>
+      </c>
+      <c r="H311" t="s">
+        <v>17</v>
+      </c>
+      <c r="J311">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>416</v>
+      </c>
+      <c r="B312" t="s">
+        <v>479</v>
+      </c>
+      <c r="C312" t="s">
+        <v>61</v>
+      </c>
+      <c r="D312">
+        <v>2491</v>
+      </c>
+      <c r="E312" t="s">
+        <v>391</v>
+      </c>
+      <c r="F312" t="s">
+        <v>67</v>
+      </c>
+      <c r="G312">
+        <v>20251005</v>
+      </c>
+      <c r="H312" t="s">
+        <v>17</v>
+      </c>
+      <c r="J312">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>417</v>
+      </c>
+      <c r="B313" t="s">
+        <v>480</v>
+      </c>
+      <c r="C313" t="s">
+        <v>62</v>
+      </c>
+      <c r="D313">
+        <v>2491</v>
+      </c>
+      <c r="E313" t="s">
+        <v>138</v>
+      </c>
+      <c r="F313" t="s">
+        <v>66</v>
+      </c>
+      <c r="G313">
+        <v>20251005</v>
+      </c>
+      <c r="H313" t="s">
+        <v>17</v>
+      </c>
+      <c r="J313">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>383</v>
+      </c>
+      <c r="B314" t="s">
+        <v>481</v>
+      </c>
+      <c r="C314" t="s">
+        <v>63</v>
+      </c>
+      <c r="D314">
+        <v>2491</v>
+      </c>
+      <c r="E314" t="s">
+        <v>24</v>
+      </c>
+      <c r="F314" t="s">
+        <v>66</v>
+      </c>
+      <c r="G314">
+        <v>20251005</v>
+      </c>
+      <c r="H314" t="s">
+        <v>17</v>
+      </c>
+      <c r="J314">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>389</v>
+      </c>
+      <c r="B315" t="s">
+        <v>482</v>
+      </c>
+      <c r="C315" t="s">
+        <v>65</v>
+      </c>
+      <c r="D315">
+        <v>2489</v>
+      </c>
+      <c r="E315" t="s">
+        <v>102</v>
+      </c>
+      <c r="F315" t="s">
+        <v>66</v>
+      </c>
+      <c r="G315">
+        <v>20251005</v>
+      </c>
+      <c r="H315" t="s">
+        <v>17</v>
+      </c>
+      <c r="J315">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>385</v>
+      </c>
+      <c r="B316" t="s">
+        <v>483</v>
+      </c>
+      <c r="C316" t="s">
+        <v>60</v>
+      </c>
+      <c r="D316">
+        <v>2489</v>
+      </c>
+      <c r="E316" t="s">
+        <v>84</v>
+      </c>
+      <c r="F316" t="s">
+        <v>67</v>
+      </c>
+      <c r="G316">
+        <v>20251005</v>
+      </c>
+      <c r="H316" t="s">
+        <v>17</v>
+      </c>
+      <c r="J316">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>386</v>
+      </c>
+      <c r="B317" t="s">
+        <v>484</v>
+      </c>
+      <c r="C317" t="s">
+        <v>63</v>
+      </c>
+      <c r="D317">
+        <v>2489</v>
+      </c>
+      <c r="E317" t="s">
+        <v>395</v>
+      </c>
+      <c r="F317" t="s">
+        <v>67</v>
+      </c>
+      <c r="G317">
+        <v>20251005</v>
+      </c>
+      <c r="H317" t="s">
+        <v>17</v>
+      </c>
+      <c r="J317">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>387</v>
+      </c>
+      <c r="B318" t="s">
+        <v>485</v>
+      </c>
+      <c r="C318" t="s">
+        <v>62</v>
+      </c>
+      <c r="D318">
+        <v>2489</v>
+      </c>
+      <c r="E318" t="s">
+        <v>507</v>
+      </c>
+      <c r="F318" t="s">
+        <v>66</v>
+      </c>
+      <c r="G318">
+        <v>20251005</v>
+      </c>
+      <c r="H318" t="s">
+        <v>17</v>
+      </c>
+      <c r="J318">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>388</v>
+      </c>
+      <c r="B319" t="s">
+        <v>486</v>
+      </c>
+      <c r="C319" t="s">
+        <v>63</v>
+      </c>
+      <c r="D319">
+        <v>2489</v>
+      </c>
+      <c r="E319" t="s">
+        <v>99</v>
+      </c>
+      <c r="F319" t="s">
+        <v>67</v>
+      </c>
+      <c r="G319">
+        <v>20251005</v>
+      </c>
+      <c r="H319" t="s">
+        <v>17</v>
+      </c>
+      <c r="J319">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>389</v>
+      </c>
+      <c r="B320" t="s">
+        <v>487</v>
+      </c>
+      <c r="C320" t="s">
+        <v>61</v>
+      </c>
+      <c r="D320">
+        <v>2489</v>
+      </c>
+      <c r="E320" t="s">
+        <v>508</v>
+      </c>
+      <c r="F320" t="s">
+        <v>67</v>
+      </c>
+      <c r="G320">
+        <v>20251005</v>
+      </c>
+      <c r="H320" t="s">
+        <v>17</v>
+      </c>
+      <c r="J320">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>391</v>
+      </c>
+      <c r="B321" t="s">
+        <v>488</v>
+      </c>
+      <c r="C321" t="s">
+        <v>64</v>
+      </c>
+      <c r="D321">
+        <v>2489</v>
+      </c>
+      <c r="E321" t="s">
+        <v>99</v>
+      </c>
+      <c r="F321" t="s">
+        <v>67</v>
+      </c>
+      <c r="G321">
+        <v>20251005</v>
+      </c>
+      <c r="H321" t="s">
+        <v>17</v>
+      </c>
+      <c r="J321">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>392</v>
+      </c>
+      <c r="B322" t="s">
+        <v>489</v>
+      </c>
+      <c r="C322" t="s">
+        <v>62</v>
+      </c>
+      <c r="D322">
+        <v>2489</v>
+      </c>
+      <c r="E322" t="s">
+        <v>86</v>
+      </c>
+      <c r="F322" t="s">
+        <v>67</v>
+      </c>
+      <c r="G322">
+        <v>20251005</v>
+      </c>
+      <c r="H322" t="s">
+        <v>17</v>
+      </c>
+      <c r="J322">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <v>393</v>
+      </c>
+      <c r="B323" t="s">
+        <v>490</v>
+      </c>
+      <c r="C323" t="s">
+        <v>65</v>
+      </c>
+      <c r="D323">
+        <v>2489</v>
+      </c>
+      <c r="E323" t="s">
+        <v>99</v>
+      </c>
+      <c r="F323" t="s">
+        <v>67</v>
+      </c>
+      <c r="G323">
+        <v>20251005</v>
+      </c>
+      <c r="H323" t="s">
+        <v>17</v>
+      </c>
+      <c r="J323">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <v>320</v>
+      </c>
+      <c r="B324" t="s">
+        <v>491</v>
+      </c>
+      <c r="C324" t="s">
+        <v>65</v>
+      </c>
+      <c r="D324">
+        <v>2489</v>
+      </c>
+      <c r="E324" t="s">
+        <v>509</v>
+      </c>
+      <c r="F324" t="s">
+        <v>66</v>
+      </c>
+      <c r="G324">
+        <v>20251005</v>
+      </c>
+      <c r="H324" t="s">
+        <v>17</v>
+      </c>
+      <c r="J324">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <v>302</v>
+      </c>
+      <c r="D325">
+        <v>2489</v>
+      </c>
+      <c r="F325" t="s">
+        <v>67</v>
+      </c>
+      <c r="G325">
+        <v>20251005</v>
+      </c>
+      <c r="H325" t="s">
+        <v>17</v>
+      </c>
+      <c r="J325">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <v>305</v>
+      </c>
+      <c r="B326" t="s">
+        <v>492</v>
+      </c>
+      <c r="C326" t="s">
+        <v>59</v>
+      </c>
+      <c r="D326">
+        <v>2474</v>
+      </c>
+      <c r="E326" t="s">
+        <v>86</v>
+      </c>
+      <c r="F326" t="s">
+        <v>67</v>
+      </c>
+      <c r="G326">
+        <v>20251005</v>
+      </c>
+      <c r="H326" t="s">
+        <v>17</v>
+      </c>
+      <c r="J326">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A327">
+        <v>306</v>
+      </c>
+      <c r="B327" t="s">
+        <v>493</v>
+      </c>
+      <c r="C327" t="s">
+        <v>61</v>
+      </c>
+      <c r="D327">
+        <v>2474</v>
+      </c>
+      <c r="E327" t="s">
+        <v>202</v>
+      </c>
+      <c r="F327" t="s">
+        <v>66</v>
+      </c>
+      <c r="G327">
+        <v>20251005</v>
+      </c>
+      <c r="H327" t="s">
+        <v>17</v>
+      </c>
+      <c r="J327">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A328">
+        <v>307</v>
+      </c>
+      <c r="B328" t="s">
+        <v>494</v>
+      </c>
+      <c r="C328" t="s">
+        <v>62</v>
+      </c>
+      <c r="D328">
+        <v>2474</v>
+      </c>
+      <c r="E328" t="s">
+        <v>86</v>
+      </c>
+      <c r="F328" t="s">
+        <v>67</v>
+      </c>
+      <c r="G328">
+        <v>20251005</v>
+      </c>
+      <c r="H328" t="s">
+        <v>17</v>
+      </c>
+      <c r="J328">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A329">
+        <v>309</v>
+      </c>
+      <c r="B329" t="s">
+        <v>479</v>
+      </c>
+      <c r="C329" t="s">
+        <v>64</v>
+      </c>
+      <c r="D329">
+        <v>2474</v>
+      </c>
+      <c r="E329" t="s">
+        <v>309</v>
+      </c>
+      <c r="F329" t="s">
+        <v>66</v>
+      </c>
+      <c r="G329">
+        <v>20251005</v>
+      </c>
+      <c r="H329" t="s">
+        <v>17</v>
+      </c>
+      <c r="J329">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A330">
+        <v>311</v>
+      </c>
+      <c r="B330" t="s">
+        <v>495</v>
+      </c>
+      <c r="C330" t="s">
+        <v>65</v>
+      </c>
+      <c r="D330">
+        <v>2474</v>
+      </c>
+      <c r="E330" t="s">
+        <v>395</v>
+      </c>
+      <c r="F330" t="s">
+        <v>66</v>
+      </c>
+      <c r="G330">
+        <v>20251005</v>
+      </c>
+      <c r="H330" t="s">
+        <v>17</v>
+      </c>
+      <c r="J330">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A331">
+        <v>310</v>
+      </c>
+      <c r="B331" t="s">
+        <v>496</v>
+      </c>
+      <c r="C331" t="s">
+        <v>64</v>
+      </c>
+      <c r="D331">
+        <v>2474</v>
+      </c>
+      <c r="E331" t="s">
+        <v>84</v>
+      </c>
+      <c r="F331" t="s">
+        <v>67</v>
+      </c>
+      <c r="G331">
+        <v>20251005</v>
+      </c>
+      <c r="H331" t="s">
+        <v>17</v>
+      </c>
+      <c r="J331">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A332">
+        <v>312</v>
+      </c>
+      <c r="B332" t="s">
+        <v>497</v>
+      </c>
+      <c r="C332" t="s">
+        <v>59</v>
+      </c>
+      <c r="D332">
+        <v>2474</v>
+      </c>
+      <c r="E332" t="s">
+        <v>136</v>
+      </c>
+      <c r="F332" t="s">
+        <v>66</v>
+      </c>
+      <c r="G332">
+        <v>20251005</v>
+      </c>
+      <c r="H332" t="s">
+        <v>17</v>
+      </c>
+      <c r="J332">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <v>313</v>
+      </c>
+      <c r="B333" t="s">
+        <v>498</v>
+      </c>
+      <c r="C333" t="s">
+        <v>60</v>
+      </c>
+      <c r="D333">
+        <v>2474</v>
+      </c>
+      <c r="E333" t="s">
+        <v>102</v>
+      </c>
+      <c r="F333" t="s">
+        <v>66</v>
+      </c>
+      <c r="G333">
+        <v>20251005</v>
+      </c>
+      <c r="H333" t="s">
+        <v>17</v>
+      </c>
+      <c r="J333">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A334">
+        <v>314</v>
+      </c>
+      <c r="B334" t="s">
+        <v>499</v>
+      </c>
+      <c r="C334" t="s">
+        <v>61</v>
+      </c>
+      <c r="D334">
+        <v>2474</v>
+      </c>
+      <c r="E334" t="s">
+        <v>86</v>
+      </c>
+      <c r="F334" t="s">
+        <v>67</v>
+      </c>
+      <c r="G334">
+        <v>20251005</v>
+      </c>
+      <c r="H334" t="s">
+        <v>17</v>
+      </c>
+      <c r="J334">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A335">
+        <v>315</v>
+      </c>
+      <c r="B335" t="s">
+        <v>500</v>
+      </c>
+      <c r="C335" t="s">
+        <v>64</v>
+      </c>
+      <c r="D335">
+        <v>2474</v>
+      </c>
+      <c r="E335" t="s">
+        <v>419</v>
+      </c>
+      <c r="F335" t="s">
+        <v>66</v>
+      </c>
+      <c r="G335">
+        <v>20251005</v>
+      </c>
+      <c r="H335" t="s">
+        <v>17</v>
+      </c>
+      <c r="J335">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A336">
+        <v>316</v>
+      </c>
+      <c r="B336" t="s">
+        <v>501</v>
+      </c>
+      <c r="C336" t="s">
+        <v>63</v>
+      </c>
+      <c r="D336">
+        <v>2474</v>
+      </c>
+      <c r="E336" t="s">
+        <v>510</v>
+      </c>
+      <c r="F336" t="s">
+        <v>66</v>
+      </c>
+      <c r="G336">
+        <v>20251005</v>
+      </c>
+      <c r="H336" t="s">
+        <v>17</v>
+      </c>
+      <c r="J336">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A337">
+        <v>317</v>
+      </c>
+      <c r="B337" t="s">
+        <v>502</v>
+      </c>
+      <c r="C337" t="s">
+        <v>62</v>
+      </c>
+      <c r="D337">
+        <v>2474</v>
+      </c>
+      <c r="E337" t="s">
+        <v>511</v>
+      </c>
+      <c r="F337" t="s">
+        <v>66</v>
+      </c>
+      <c r="G337">
+        <v>20251005</v>
+      </c>
+      <c r="H337" t="s">
+        <v>17</v>
+      </c>
+      <c r="J337">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A338">
+        <v>318</v>
+      </c>
+      <c r="B338" t="s">
+        <v>503</v>
+      </c>
+      <c r="C338" t="s">
+        <v>63</v>
+      </c>
+      <c r="D338">
+        <v>2474</v>
+      </c>
+      <c r="E338" t="s">
+        <v>24</v>
+      </c>
+      <c r="F338" t="s">
+        <v>66</v>
+      </c>
+      <c r="G338">
+        <v>20251005</v>
+      </c>
+      <c r="H338" t="s">
+        <v>17</v>
+      </c>
+      <c r="J338">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
+        <v>472</v>
+      </c>
+      <c r="B339" t="s">
+        <v>504</v>
+      </c>
+      <c r="C339" t="s">
+        <v>65</v>
+      </c>
+      <c r="D339">
+        <v>2474</v>
+      </c>
+      <c r="E339" t="s">
+        <v>139</v>
+      </c>
+      <c r="F339" t="s">
+        <v>66</v>
+      </c>
+      <c r="G339">
+        <v>20251005</v>
+      </c>
+      <c r="H339" t="s">
+        <v>17</v>
+      </c>
+      <c r="J339">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A340">
+        <v>276</v>
+      </c>
+      <c r="B340" t="s">
+        <v>512</v>
+      </c>
+      <c r="C340" t="s">
+        <v>64</v>
+      </c>
+      <c r="D340">
+        <v>1467</v>
+      </c>
+      <c r="E340" t="s">
+        <v>82</v>
+      </c>
+      <c r="F340" t="s">
+        <v>67</v>
+      </c>
+      <c r="G340">
+        <v>20251005</v>
+      </c>
+      <c r="H340" t="s">
+        <v>17</v>
+      </c>
+      <c r="J340">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A341">
+        <v>272</v>
+      </c>
+      <c r="B341" t="s">
+        <v>513</v>
+      </c>
+      <c r="C341" t="s">
+        <v>59</v>
+      </c>
+      <c r="D341">
+        <v>1467</v>
+      </c>
+      <c r="E341" t="s">
+        <v>86</v>
+      </c>
+      <c r="F341" t="s">
+        <v>67</v>
+      </c>
+      <c r="G341">
+        <v>20251006</v>
+      </c>
+      <c r="H341" t="s">
+        <v>17</v>
+      </c>
+      <c r="J341">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A342">
+        <v>199</v>
+      </c>
+      <c r="B342" t="s">
+        <v>514</v>
+      </c>
+      <c r="C342" t="s">
+        <v>59</v>
+      </c>
+      <c r="D342">
+        <v>1467</v>
+      </c>
+      <c r="E342" t="s">
+        <v>202</v>
+      </c>
+      <c r="F342" t="s">
+        <v>66</v>
+      </c>
+      <c r="G342">
+        <v>20251007</v>
+      </c>
+      <c r="H342" t="s">
+        <v>17</v>
+      </c>
+      <c r="J342">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A343">
+        <v>278</v>
+      </c>
+      <c r="B343" t="s">
+        <v>515</v>
+      </c>
+      <c r="C343" t="s">
+        <v>64</v>
+      </c>
+      <c r="D343">
+        <v>1467</v>
+      </c>
+      <c r="E343" t="s">
+        <v>506</v>
+      </c>
+      <c r="F343" t="s">
+        <v>66</v>
+      </c>
+      <c r="G343">
+        <v>20251008</v>
+      </c>
+      <c r="H343" t="s">
+        <v>17</v>
+      </c>
+      <c r="J343">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A344">
+        <v>279</v>
+      </c>
+      <c r="B344" t="s">
+        <v>516</v>
+      </c>
+      <c r="C344" t="s">
+        <v>65</v>
+      </c>
+      <c r="D344">
+        <v>1467</v>
+      </c>
+      <c r="E344" t="s">
+        <v>24</v>
+      </c>
+      <c r="F344" t="s">
+        <v>66</v>
+      </c>
+      <c r="G344">
+        <v>20251009</v>
+      </c>
+      <c r="H344" t="s">
+        <v>17</v>
+      </c>
+      <c r="J344">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A345">
+        <v>280</v>
+      </c>
+      <c r="B345" t="s">
+        <v>517</v>
+      </c>
+      <c r="C345" t="s">
+        <v>61</v>
+      </c>
+      <c r="D345">
+        <v>1467</v>
+      </c>
+      <c r="E345" t="s">
+        <v>138</v>
+      </c>
+      <c r="F345" t="s">
+        <v>66</v>
+      </c>
+      <c r="G345">
+        <v>20251010</v>
+      </c>
+      <c r="H345" t="s">
+        <v>17</v>
+      </c>
+      <c r="J345">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A346">
+        <v>281</v>
+      </c>
+      <c r="B346" t="s">
+        <v>518</v>
+      </c>
+      <c r="C346" t="s">
+        <v>60</v>
+      </c>
+      <c r="D346">
+        <v>1467</v>
+      </c>
+      <c r="E346" t="s">
+        <v>526</v>
+      </c>
+      <c r="F346" t="s">
+        <v>67</v>
+      </c>
+      <c r="G346">
+        <v>20251011</v>
+      </c>
+      <c r="H346" t="s">
+        <v>17</v>
+      </c>
+      <c r="J346">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A347">
+        <v>191</v>
+      </c>
+      <c r="B347" t="s">
+        <v>519</v>
+      </c>
+      <c r="C347" t="s">
+        <v>65</v>
+      </c>
+      <c r="D347">
+        <v>1467</v>
+      </c>
+      <c r="E347" t="s">
+        <v>24</v>
+      </c>
+      <c r="F347" t="s">
+        <v>66</v>
+      </c>
+      <c r="G347">
+        <v>20251012</v>
+      </c>
+      <c r="H347" t="s">
+        <v>17</v>
+      </c>
+      <c r="J347">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A348">
+        <v>291</v>
+      </c>
+      <c r="B348" t="s">
+        <v>520</v>
+      </c>
+      <c r="C348" t="s">
+        <v>63</v>
+      </c>
+      <c r="D348">
+        <v>1467</v>
+      </c>
+      <c r="E348" t="s">
+        <v>73</v>
+      </c>
+      <c r="F348" t="s">
+        <v>66</v>
+      </c>
+      <c r="G348">
+        <v>20251013</v>
+      </c>
+      <c r="H348" t="s">
+        <v>17</v>
+      </c>
+      <c r="J348">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A349">
+        <v>193</v>
+      </c>
+      <c r="B349" t="s">
+        <v>521</v>
+      </c>
+      <c r="C349" t="s">
+        <v>64</v>
+      </c>
+      <c r="D349">
+        <v>1467</v>
+      </c>
+      <c r="E349" t="s">
+        <v>527</v>
+      </c>
+      <c r="F349" t="s">
+        <v>66</v>
+      </c>
+      <c r="G349">
+        <v>20251014</v>
+      </c>
+      <c r="H349" t="s">
+        <v>17</v>
+      </c>
+      <c r="J349">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A350">
+        <v>192</v>
+      </c>
+      <c r="B350" t="s">
+        <v>522</v>
+      </c>
+      <c r="C350" t="s">
+        <v>62</v>
+      </c>
+      <c r="D350">
+        <v>1467</v>
+      </c>
+      <c r="E350" t="s">
+        <v>24</v>
+      </c>
+      <c r="F350" t="s">
+        <v>66</v>
+      </c>
+      <c r="G350">
+        <v>20251015</v>
+      </c>
+      <c r="H350" t="s">
+        <v>17</v>
+      </c>
+      <c r="J350">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A351">
+        <v>194</v>
+      </c>
+      <c r="B351" t="s">
+        <v>523</v>
+      </c>
+      <c r="C351" t="s">
+        <v>60</v>
+      </c>
+      <c r="D351">
+        <v>1467</v>
+      </c>
+      <c r="E351" t="s">
+        <v>24</v>
+      </c>
+      <c r="F351" t="s">
+        <v>66</v>
+      </c>
+      <c r="G351">
+        <v>20251016</v>
+      </c>
+      <c r="H351" t="s">
+        <v>17</v>
+      </c>
+      <c r="J351">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A352">
+        <v>195</v>
+      </c>
+      <c r="B352" t="s">
+        <v>524</v>
+      </c>
+      <c r="C352" t="s">
+        <v>61</v>
+      </c>
+      <c r="D352">
+        <v>1467</v>
+      </c>
+      <c r="E352" t="s">
+        <v>528</v>
+      </c>
+      <c r="F352" t="s">
+        <v>67</v>
+      </c>
+      <c r="G352">
+        <v>20251017</v>
+      </c>
+      <c r="H352" t="s">
+        <v>17</v>
+      </c>
+      <c r="J352">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A353">
+        <v>196</v>
+      </c>
+      <c r="B353" t="s">
+        <v>525</v>
+      </c>
+      <c r="C353" t="s">
+        <v>63</v>
+      </c>
+      <c r="D353">
+        <v>1467</v>
+      </c>
+      <c r="E353" t="s">
+        <v>260</v>
+      </c>
+      <c r="F353" t="s">
+        <v>66</v>
+      </c>
+      <c r="G353">
+        <v>20251018</v>
+      </c>
+      <c r="H353" t="s">
+        <v>17</v>
+      </c>
+      <c r="J353">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:P353" xr:uid="{859618DA-7D2E-F14A-9531-A0F7323C3157}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L105">
     <sortCondition ref="C2:C105"/>
   </sortState>

</xml_diff>